<commit_message>
Lots of UI and server-side bigfixes, enhanced recognition for postal tuition timetable type, fresh DB updates
</commit_message>
<xml_diff>
--- a/www/tests/parser/TestPostalTutorials.xlsx
+++ b/www/tests/parser/TestPostalTutorials.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="232">
   <si>
     <t>"Утверждаю"</t>
   </si>
@@ -706,21 +706,13 @@
     <t>с 18:00</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Теория автом. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="8"/>
-        <rFont val="Arial Cyr"/>
-        <charset val="204"/>
-      </rPr>
-      <t>c 18:00</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">15.04,13.05(3ч)   </t>
+  </si>
+  <si>
+    <t>Теория автом.</t>
+  </si>
+  <si>
+    <t>c 18:00</t>
   </si>
 </sst>
 </file>
@@ -2304,6 +2296,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2312,6 +2334,309 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2322,30 +2647,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2354,21 +2655,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2384,300 +2670,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2987,8 +2979,8 @@
   </sheetPr>
   <dimension ref="A1:AE108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="X29" sqref="X29:AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3172,42 +3164,42 @@
       <c r="G9" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="H9" s="327" t="s">
+      <c r="H9" s="429" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="318"/>
-      <c r="J9" s="318"/>
-      <c r="K9" s="319"/>
-      <c r="L9" s="317" t="s">
+      <c r="I9" s="425"/>
+      <c r="J9" s="425"/>
+      <c r="K9" s="426"/>
+      <c r="L9" s="424" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="318"/>
-      <c r="N9" s="318"/>
-      <c r="O9" s="319"/>
-      <c r="P9" s="317" t="s">
+      <c r="M9" s="425"/>
+      <c r="N9" s="425"/>
+      <c r="O9" s="426"/>
+      <c r="P9" s="424" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="328"/>
-      <c r="R9" s="328"/>
-      <c r="S9" s="329"/>
-      <c r="T9" s="327" t="s">
+      <c r="Q9" s="430"/>
+      <c r="R9" s="430"/>
+      <c r="S9" s="431"/>
+      <c r="T9" s="429" t="s">
         <v>19</v>
       </c>
-      <c r="U9" s="318"/>
-      <c r="V9" s="318"/>
-      <c r="W9" s="319"/>
-      <c r="X9" s="317" t="s">
+      <c r="U9" s="425"/>
+      <c r="V9" s="425"/>
+      <c r="W9" s="426"/>
+      <c r="X9" s="424" t="s">
         <v>20</v>
       </c>
-      <c r="Y9" s="318"/>
-      <c r="Z9" s="318"/>
-      <c r="AA9" s="319"/>
-      <c r="AB9" s="317" t="s">
+      <c r="Y9" s="425"/>
+      <c r="Z9" s="425"/>
+      <c r="AA9" s="426"/>
+      <c r="AB9" s="424" t="s">
         <v>21</v>
       </c>
-      <c r="AC9" s="318"/>
-      <c r="AD9" s="318"/>
-      <c r="AE9" s="319"/>
+      <c r="AC9" s="425"/>
+      <c r="AD9" s="425"/>
+      <c r="AE9" s="426"/>
     </row>
     <row r="10" spans="1:31" s="20" customFormat="1" ht="26.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="14"/>
@@ -3256,40 +3248,40 @@
       <c r="G11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="321" t="s">
+      <c r="H11" s="329" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="322"/>
-      <c r="J11" s="322"/>
-      <c r="K11" s="322"/>
+      <c r="I11" s="330"/>
+      <c r="J11" s="330"/>
+      <c r="K11" s="330"/>
       <c r="L11" s="323" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="322"/>
-      <c r="N11" s="322"/>
-      <c r="O11" s="324"/>
-      <c r="P11" s="325" t="s">
+      <c r="M11" s="330"/>
+      <c r="N11" s="330"/>
+      <c r="O11" s="331"/>
+      <c r="P11" s="427" t="s">
         <v>25</v>
       </c>
-      <c r="Q11" s="326"/>
-      <c r="R11" s="303" t="s">
+      <c r="Q11" s="428"/>
+      <c r="R11" s="313" t="s">
         <v>26</v>
       </c>
-      <c r="S11" s="305"/>
-      <c r="T11" s="303"/>
-      <c r="U11" s="304"/>
-      <c r="V11" s="304"/>
-      <c r="W11" s="305"/>
-      <c r="X11" s="306"/>
-      <c r="Y11" s="307"/>
-      <c r="Z11" s="307"/>
-      <c r="AA11" s="308"/>
-      <c r="AB11" s="309" t="s">
+      <c r="S11" s="315"/>
+      <c r="T11" s="313"/>
+      <c r="U11" s="314"/>
+      <c r="V11" s="314"/>
+      <c r="W11" s="315"/>
+      <c r="X11" s="421"/>
+      <c r="Y11" s="422"/>
+      <c r="Z11" s="422"/>
+      <c r="AA11" s="423"/>
+      <c r="AB11" s="354" t="s">
         <v>27</v>
       </c>
-      <c r="AC11" s="310"/>
-      <c r="AD11" s="310"/>
-      <c r="AE11" s="311"/>
+      <c r="AC11" s="401"/>
+      <c r="AD11" s="401"/>
+      <c r="AE11" s="402"/>
     </row>
     <row r="12" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
@@ -3323,18 +3315,18 @@
       <c r="Q12" s="34"/>
       <c r="R12" s="31"/>
       <c r="S12" s="35"/>
-      <c r="T12" s="312"/>
-      <c r="U12" s="313"/>
-      <c r="V12" s="313"/>
-      <c r="W12" s="314"/>
+      <c r="T12" s="393"/>
+      <c r="U12" s="394"/>
+      <c r="V12" s="394"/>
+      <c r="W12" s="395"/>
       <c r="X12" s="36"/>
       <c r="Y12" s="31"/>
       <c r="Z12" s="37"/>
       <c r="AA12" s="38"/>
-      <c r="AB12" s="315"/>
-      <c r="AC12" s="316"/>
-      <c r="AD12" s="316"/>
-      <c r="AE12" s="320"/>
+      <c r="AB12" s="416"/>
+      <c r="AC12" s="417"/>
+      <c r="AD12" s="417"/>
+      <c r="AE12" s="418"/>
     </row>
     <row r="13" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -3358,28 +3350,28 @@
       <c r="M13" s="41"/>
       <c r="N13" s="27"/>
       <c r="O13" s="42"/>
-      <c r="P13" s="338" t="s">
+      <c r="P13" s="306" t="s">
         <v>32</v>
       </c>
-      <c r="Q13" s="339"/>
-      <c r="R13" s="338" t="s">
+      <c r="Q13" s="312"/>
+      <c r="R13" s="306" t="s">
         <v>33</v>
       </c>
-      <c r="S13" s="339"/>
-      <c r="T13" s="338"/>
-      <c r="U13" s="340"/>
-      <c r="V13" s="340"/>
-      <c r="W13" s="339"/>
+      <c r="S13" s="312"/>
+      <c r="T13" s="306"/>
+      <c r="U13" s="307"/>
+      <c r="V13" s="307"/>
+      <c r="W13" s="312"/>
       <c r="X13" s="44"/>
-      <c r="Y13" s="341"/>
-      <c r="Z13" s="341"/>
-      <c r="AA13" s="342"/>
-      <c r="AB13" s="343" t="s">
+      <c r="Y13" s="419"/>
+      <c r="Z13" s="419"/>
+      <c r="AA13" s="420"/>
+      <c r="AB13" s="342" t="s">
         <v>34</v>
       </c>
-      <c r="AC13" s="336"/>
-      <c r="AD13" s="336"/>
-      <c r="AE13" s="344"/>
+      <c r="AC13" s="318"/>
+      <c r="AD13" s="318"/>
+      <c r="AE13" s="357"/>
     </row>
     <row r="14" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -3405,12 +3397,12 @@
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="32"/>
-      <c r="L14" s="330" t="s">
+      <c r="L14" s="341" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="331"/>
-      <c r="N14" s="331"/>
-      <c r="O14" s="331"/>
+      <c r="M14" s="310"/>
+      <c r="N14" s="310"/>
+      <c r="O14" s="310"/>
       <c r="P14" s="33"/>
       <c r="Q14" s="46"/>
       <c r="R14" s="31"/>
@@ -3421,14 +3413,14 @@
       <c r="W14" s="35"/>
       <c r="X14" s="44"/>
       <c r="Y14" s="37"/>
-      <c r="Z14" s="332"/>
-      <c r="AA14" s="333"/>
-      <c r="AB14" s="334" t="s">
+      <c r="Z14" s="414"/>
+      <c r="AA14" s="415"/>
+      <c r="AB14" s="309" t="s">
         <v>39</v>
       </c>
-      <c r="AC14" s="331"/>
-      <c r="AD14" s="331"/>
-      <c r="AE14" s="335"/>
+      <c r="AC14" s="310"/>
+      <c r="AD14" s="310"/>
+      <c r="AE14" s="408"/>
     </row>
     <row r="15" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
@@ -3452,10 +3444,10 @@
       <c r="Q15" s="56"/>
       <c r="R15" s="53"/>
       <c r="S15" s="35"/>
-      <c r="T15" s="334"/>
-      <c r="U15" s="336"/>
-      <c r="V15" s="336"/>
-      <c r="W15" s="337"/>
+      <c r="T15" s="309"/>
+      <c r="U15" s="318"/>
+      <c r="V15" s="318"/>
+      <c r="W15" s="319"/>
       <c r="X15" s="57"/>
       <c r="Z15" s="58"/>
       <c r="AA15" s="59"/>
@@ -3529,44 +3521,44 @@
       <c r="G17" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="430" t="s">
+      <c r="H17" s="304" t="s">
         <v>48</v>
       </c>
       <c r="I17" s="301"/>
       <c r="J17" s="301"/>
       <c r="K17" s="302"/>
-      <c r="L17" s="429" t="s">
+      <c r="L17" s="303" t="s">
         <v>48</v>
       </c>
       <c r="M17" s="301"/>
       <c r="N17" s="301"/>
       <c r="O17" s="302"/>
-      <c r="P17" s="345" t="s">
+      <c r="P17" s="339" t="s">
         <v>49</v>
       </c>
-      <c r="Q17" s="346"/>
-      <c r="R17" s="346"/>
-      <c r="S17" s="347"/>
-      <c r="T17" s="303" t="s">
+      <c r="Q17" s="326"/>
+      <c r="R17" s="326"/>
+      <c r="S17" s="344"/>
+      <c r="T17" s="313" t="s">
         <v>50</v>
       </c>
-      <c r="U17" s="305"/>
-      <c r="V17" s="303" t="s">
+      <c r="U17" s="315"/>
+      <c r="V17" s="313" t="s">
         <v>51</v>
       </c>
-      <c r="W17" s="305"/>
-      <c r="X17" s="345" t="s">
+      <c r="W17" s="315"/>
+      <c r="X17" s="339" t="s">
         <v>52</v>
       </c>
-      <c r="Y17" s="346"/>
-      <c r="Z17" s="346"/>
-      <c r="AA17" s="347"/>
-      <c r="AB17" s="309" t="s">
+      <c r="Y17" s="326"/>
+      <c r="Z17" s="326"/>
+      <c r="AA17" s="344"/>
+      <c r="AB17" s="354" t="s">
         <v>53</v>
       </c>
-      <c r="AC17" s="310"/>
-      <c r="AD17" s="310"/>
-      <c r="AE17" s="311"/>
+      <c r="AC17" s="401"/>
+      <c r="AD17" s="401"/>
+      <c r="AE17" s="402"/>
     </row>
     <row r="18" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -3602,20 +3594,20 @@
       <c r="S18" s="35"/>
       <c r="T18" s="33"/>
       <c r="U18" s="34"/>
-      <c r="V18" s="312" t="s">
+      <c r="V18" s="393" t="s">
         <v>55</v>
       </c>
-      <c r="W18" s="314"/>
-      <c r="X18" s="348" t="s">
+      <c r="W18" s="395"/>
+      <c r="X18" s="403" t="s">
         <v>56</v>
       </c>
-      <c r="Y18" s="349"/>
-      <c r="Z18" s="349"/>
-      <c r="AA18" s="350"/>
-      <c r="AB18" s="315"/>
-      <c r="AC18" s="316"/>
-      <c r="AD18" s="316"/>
-      <c r="AE18" s="320"/>
+      <c r="Y18" s="404"/>
+      <c r="Z18" s="404"/>
+      <c r="AA18" s="405"/>
+      <c r="AB18" s="416"/>
+      <c r="AC18" s="417"/>
+      <c r="AD18" s="417"/>
+      <c r="AE18" s="418"/>
     </row>
     <row r="19" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
@@ -3639,32 +3631,32 @@
       <c r="M19" s="41"/>
       <c r="N19" s="27"/>
       <c r="O19" s="42"/>
-      <c r="P19" s="338" t="s">
+      <c r="P19" s="306" t="s">
         <v>59</v>
       </c>
-      <c r="Q19" s="340"/>
-      <c r="R19" s="340"/>
-      <c r="S19" s="339"/>
-      <c r="T19" s="355" t="s">
+      <c r="Q19" s="307"/>
+      <c r="R19" s="307"/>
+      <c r="S19" s="312"/>
+      <c r="T19" s="409" t="s">
         <v>60</v>
       </c>
-      <c r="U19" s="356"/>
-      <c r="V19" s="357" t="s">
+      <c r="U19" s="410"/>
+      <c r="V19" s="411" t="s">
         <v>61</v>
       </c>
-      <c r="W19" s="358"/>
-      <c r="X19" s="338" t="s">
+      <c r="W19" s="412"/>
+      <c r="X19" s="306" t="s">
         <v>62</v>
       </c>
-      <c r="Y19" s="340"/>
-      <c r="Z19" s="340"/>
-      <c r="AA19" s="339"/>
-      <c r="AB19" s="343" t="s">
+      <c r="Y19" s="307"/>
+      <c r="Z19" s="307"/>
+      <c r="AA19" s="312"/>
+      <c r="AB19" s="342" t="s">
         <v>63</v>
       </c>
-      <c r="AC19" s="336"/>
-      <c r="AD19" s="336"/>
-      <c r="AE19" s="344"/>
+      <c r="AC19" s="318"/>
+      <c r="AD19" s="318"/>
+      <c r="AE19" s="357"/>
     </row>
     <row r="20" spans="1:31" s="79" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
@@ -3706,18 +3698,18 @@
       <c r="U20" s="46"/>
       <c r="V20" s="31"/>
       <c r="W20" s="35"/>
-      <c r="X20" s="330" t="s">
+      <c r="X20" s="341" t="s">
         <v>68</v>
       </c>
-      <c r="Y20" s="353"/>
-      <c r="Z20" s="353"/>
-      <c r="AA20" s="354"/>
-      <c r="AB20" s="330" t="s">
+      <c r="Y20" s="335"/>
+      <c r="Z20" s="335"/>
+      <c r="AA20" s="311"/>
+      <c r="AB20" s="341" t="s">
         <v>69</v>
       </c>
-      <c r="AC20" s="331"/>
-      <c r="AD20" s="331"/>
-      <c r="AE20" s="335"/>
+      <c r="AC20" s="310"/>
+      <c r="AD20" s="310"/>
+      <c r="AE20" s="408"/>
     </row>
     <row r="21" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
@@ -3790,10 +3782,10 @@
         <v>73</v>
       </c>
       <c r="U22" s="71"/>
-      <c r="V22" s="351" t="s">
+      <c r="V22" s="406" t="s">
         <v>74</v>
       </c>
-      <c r="W22" s="352"/>
+      <c r="W22" s="407"/>
       <c r="X22" s="70" t="s">
         <v>75</v>
       </c>
@@ -3819,42 +3811,42 @@
       <c r="G23" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="321" t="s">
+      <c r="H23" s="329" t="s">
         <v>80</v>
       </c>
-      <c r="I23" s="322"/>
-      <c r="J23" s="322"/>
-      <c r="K23" s="322"/>
+      <c r="I23" s="330"/>
+      <c r="J23" s="330"/>
+      <c r="K23" s="330"/>
       <c r="L23" s="323" t="s">
         <v>80</v>
       </c>
-      <c r="M23" s="322"/>
-      <c r="N23" s="322"/>
-      <c r="O23" s="324"/>
-      <c r="P23" s="345" t="s">
+      <c r="M23" s="330"/>
+      <c r="N23" s="330"/>
+      <c r="O23" s="331"/>
+      <c r="P23" s="339" t="s">
         <v>81</v>
       </c>
-      <c r="Q23" s="346"/>
-      <c r="R23" s="346"/>
-      <c r="S23" s="347"/>
-      <c r="T23" s="303" t="s">
+      <c r="Q23" s="326"/>
+      <c r="R23" s="326"/>
+      <c r="S23" s="344"/>
+      <c r="T23" s="313" t="s">
         <v>82</v>
       </c>
-      <c r="U23" s="304"/>
-      <c r="V23" s="304"/>
-      <c r="W23" s="305"/>
-      <c r="X23" s="345" t="s">
+      <c r="U23" s="314"/>
+      <c r="V23" s="314"/>
+      <c r="W23" s="315"/>
+      <c r="X23" s="339" t="s">
         <v>78</v>
       </c>
-      <c r="Y23" s="346"/>
-      <c r="Z23" s="346"/>
-      <c r="AA23" s="347"/>
-      <c r="AB23" s="359" t="s">
+      <c r="Y23" s="326"/>
+      <c r="Z23" s="326"/>
+      <c r="AA23" s="344"/>
+      <c r="AB23" s="324" t="s">
         <v>83</v>
       </c>
-      <c r="AC23" s="359"/>
-      <c r="AD23" s="359"/>
-      <c r="AE23" s="360"/>
+      <c r="AC23" s="324"/>
+      <c r="AD23" s="324"/>
+      <c r="AE23" s="413"/>
     </row>
     <row r="24" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="86" t="s">
@@ -3892,16 +3884,16 @@
       <c r="U24" s="88"/>
       <c r="V24" s="79"/>
       <c r="W24" s="89"/>
-      <c r="X24" s="312"/>
-      <c r="Y24" s="313"/>
-      <c r="Z24" s="313"/>
-      <c r="AA24" s="314"/>
-      <c r="AB24" s="336" t="s">
-        <v>230</v>
-      </c>
-      <c r="AC24" s="336"/>
-      <c r="AD24" s="336"/>
-      <c r="AE24" s="344"/>
+      <c r="X24" s="393"/>
+      <c r="Y24" s="394"/>
+      <c r="Z24" s="394"/>
+      <c r="AA24" s="395"/>
+      <c r="AB24" s="318" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC24" s="318"/>
+      <c r="AD24" s="318"/>
+      <c r="AE24" s="357"/>
     </row>
     <row r="25" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="86" t="s">
@@ -3925,30 +3917,30 @@
       <c r="M25" s="41"/>
       <c r="N25" s="27"/>
       <c r="O25" s="42"/>
-      <c r="P25" s="338" t="s">
+      <c r="P25" s="306" t="s">
         <v>87</v>
       </c>
-      <c r="Q25" s="340"/>
-      <c r="R25" s="340"/>
-      <c r="S25" s="339"/>
-      <c r="T25" s="338" t="s">
+      <c r="Q25" s="307"/>
+      <c r="R25" s="307"/>
+      <c r="S25" s="312"/>
+      <c r="T25" s="306" t="s">
         <v>88</v>
       </c>
-      <c r="U25" s="340"/>
-      <c r="V25" s="340"/>
-      <c r="W25" s="339"/>
-      <c r="X25" s="363" t="s">
+      <c r="U25" s="307"/>
+      <c r="V25" s="307"/>
+      <c r="W25" s="312"/>
+      <c r="X25" s="389" t="s">
         <v>89</v>
       </c>
-      <c r="Y25" s="364"/>
-      <c r="Z25" s="364"/>
-      <c r="AA25" s="365"/>
-      <c r="AB25" s="366" t="s">
+      <c r="Y25" s="381"/>
+      <c r="Z25" s="381"/>
+      <c r="AA25" s="390"/>
+      <c r="AB25" s="398" t="s">
         <v>90</v>
       </c>
-      <c r="AC25" s="336"/>
-      <c r="AD25" s="336"/>
-      <c r="AE25" s="344"/>
+      <c r="AC25" s="318"/>
+      <c r="AD25" s="318"/>
+      <c r="AE25" s="357"/>
     </row>
     <row r="26" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="86" t="s">
@@ -3986,22 +3978,22 @@
       </c>
       <c r="R26" s="31"/>
       <c r="S26" s="35"/>
-      <c r="T26" s="367" t="s">
+      <c r="T26" s="332" t="s">
         <v>94</v>
       </c>
-      <c r="U26" s="368"/>
-      <c r="V26" s="368"/>
-      <c r="W26" s="369"/>
-      <c r="X26" s="353" t="s">
+      <c r="U26" s="399"/>
+      <c r="V26" s="399"/>
+      <c r="W26" s="400"/>
+      <c r="X26" s="335" t="s">
         <v>92</v>
       </c>
-      <c r="Y26" s="353"/>
-      <c r="Z26" s="353"/>
-      <c r="AA26" s="354"/>
-      <c r="AB26" s="370" t="s">
+      <c r="Y26" s="335"/>
+      <c r="Z26" s="335"/>
+      <c r="AA26" s="311"/>
+      <c r="AB26" s="382" t="s">
         <v>95</v>
       </c>
-      <c r="AC26" s="371"/>
+      <c r="AC26" s="383"/>
       <c r="AD26" s="93" t="s">
         <v>79</v>
       </c>
@@ -4029,10 +4021,10 @@
       <c r="Q27" s="45"/>
       <c r="R27" s="53"/>
       <c r="S27" s="35"/>
-      <c r="T27" s="372"/>
-      <c r="U27" s="373"/>
-      <c r="V27" s="373"/>
-      <c r="W27" s="374"/>
+      <c r="T27" s="384"/>
+      <c r="U27" s="385"/>
+      <c r="V27" s="385"/>
+      <c r="W27" s="386"/>
       <c r="X27" s="57"/>
       <c r="Z27" s="58"/>
       <c r="AA27" s="59"/>
@@ -4043,9 +4035,11 @@
         <v>228</v>
       </c>
       <c r="AD27" s="99" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE27" s="100"/>
+        <v>230</v>
+      </c>
+      <c r="AE27" s="100" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="28" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="101"/>
@@ -4089,14 +4083,14 @@
       <c r="Y28" s="104"/>
       <c r="Z28" s="105"/>
       <c r="AA28" s="106"/>
-      <c r="AB28" s="375" t="s">
+      <c r="AB28" s="387" t="s">
         <v>101</v>
       </c>
-      <c r="AC28" s="376"/>
-      <c r="AD28" s="361" t="s">
+      <c r="AC28" s="388"/>
+      <c r="AD28" s="396" t="s">
         <v>102</v>
       </c>
-      <c r="AE28" s="362"/>
+      <c r="AE28" s="397"/>
     </row>
     <row r="29" spans="1:31" s="13" customFormat="1" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="86" t="s">
@@ -4110,32 +4104,32 @@
       <c r="G29" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="321" t="s">
+      <c r="H29" s="329" t="s">
         <v>104</v>
       </c>
-      <c r="I29" s="322"/>
-      <c r="J29" s="322"/>
-      <c r="K29" s="322"/>
+      <c r="I29" s="330"/>
+      <c r="J29" s="330"/>
+      <c r="K29" s="330"/>
       <c r="L29" s="323" t="s">
         <v>104</v>
       </c>
-      <c r="M29" s="322"/>
-      <c r="N29" s="322"/>
-      <c r="O29" s="324"/>
-      <c r="P29" s="345"/>
-      <c r="Q29" s="346"/>
-      <c r="R29" s="346"/>
-      <c r="S29" s="347"/>
-      <c r="T29" s="377" t="s">
+      <c r="M29" s="330"/>
+      <c r="N29" s="330"/>
+      <c r="O29" s="331"/>
+      <c r="P29" s="339"/>
+      <c r="Q29" s="326"/>
+      <c r="R29" s="326"/>
+      <c r="S29" s="344"/>
+      <c r="T29" s="391" t="s">
         <v>105</v>
       </c>
-      <c r="U29" s="378"/>
-      <c r="V29" s="378"/>
-      <c r="W29" s="378"/>
-      <c r="X29" s="345"/>
-      <c r="Y29" s="346"/>
-      <c r="Z29" s="346"/>
-      <c r="AA29" s="347"/>
+      <c r="U29" s="392"/>
+      <c r="V29" s="392"/>
+      <c r="W29" s="392"/>
+      <c r="X29" s="339"/>
+      <c r="Y29" s="326"/>
+      <c r="Z29" s="326"/>
+      <c r="AA29" s="344"/>
       <c r="AB29" s="107" t="s">
         <v>106</v>
       </c>
@@ -4171,18 +4165,18 @@
       <c r="M30" s="31"/>
       <c r="N30" s="31"/>
       <c r="O30" s="32"/>
-      <c r="P30" s="312"/>
-      <c r="Q30" s="313"/>
-      <c r="R30" s="313"/>
-      <c r="S30" s="314"/>
+      <c r="P30" s="393"/>
+      <c r="Q30" s="394"/>
+      <c r="R30" s="394"/>
+      <c r="S30" s="395"/>
       <c r="T30" s="109"/>
       <c r="U30" s="110"/>
       <c r="V30" s="28"/>
       <c r="W30" s="50"/>
-      <c r="X30" s="312"/>
-      <c r="Y30" s="313"/>
-      <c r="Z30" s="313"/>
-      <c r="AA30" s="314"/>
+      <c r="X30" s="393"/>
+      <c r="Y30" s="394"/>
+      <c r="Z30" s="394"/>
+      <c r="AA30" s="395"/>
       <c r="AB30" s="111"/>
       <c r="AC30" s="112"/>
       <c r="AD30" s="110"/>
@@ -4210,20 +4204,20 @@
       <c r="M31" s="41"/>
       <c r="N31" s="27"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="338"/>
-      <c r="Q31" s="340"/>
-      <c r="R31" s="340"/>
-      <c r="S31" s="339"/>
-      <c r="T31" s="363" t="s">
+      <c r="P31" s="306"/>
+      <c r="Q31" s="307"/>
+      <c r="R31" s="307"/>
+      <c r="S31" s="312"/>
+      <c r="T31" s="389" t="s">
         <v>109</v>
       </c>
-      <c r="U31" s="364"/>
-      <c r="V31" s="364"/>
-      <c r="W31" s="364"/>
-      <c r="X31" s="363"/>
-      <c r="Y31" s="364"/>
-      <c r="Z31" s="364"/>
-      <c r="AA31" s="365"/>
+      <c r="U31" s="381"/>
+      <c r="V31" s="381"/>
+      <c r="W31" s="381"/>
+      <c r="X31" s="389"/>
+      <c r="Y31" s="381"/>
+      <c r="Z31" s="381"/>
+      <c r="AA31" s="390"/>
       <c r="AB31" s="114"/>
       <c r="AC31" s="112" t="s">
         <v>110</v>
@@ -4261,20 +4255,20 @@
       </c>
       <c r="N32" s="31"/>
       <c r="O32" s="32"/>
-      <c r="P32" s="379"/>
-      <c r="Q32" s="380"/>
-      <c r="R32" s="380"/>
-      <c r="S32" s="381"/>
-      <c r="T32" s="382" t="s">
+      <c r="P32" s="351"/>
+      <c r="Q32" s="352"/>
+      <c r="R32" s="352"/>
+      <c r="S32" s="353"/>
+      <c r="T32" s="380" t="s">
         <v>113</v>
       </c>
-      <c r="U32" s="364"/>
-      <c r="V32" s="364"/>
-      <c r="W32" s="364"/>
-      <c r="X32" s="330"/>
-      <c r="Y32" s="331"/>
-      <c r="Z32" s="331"/>
-      <c r="AA32" s="354"/>
+      <c r="U32" s="381"/>
+      <c r="V32" s="381"/>
+      <c r="W32" s="381"/>
+      <c r="X32" s="341"/>
+      <c r="Y32" s="310"/>
+      <c r="Z32" s="310"/>
+      <c r="AA32" s="311"/>
       <c r="AB32" s="116"/>
       <c r="AC32" s="110" t="s">
         <v>114</v>
@@ -4375,34 +4369,34 @@
       <c r="G35" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="321" t="s">
+      <c r="H35" s="329" t="s">
         <v>119</v>
       </c>
-      <c r="I35" s="322"/>
-      <c r="J35" s="322"/>
-      <c r="K35" s="322"/>
+      <c r="I35" s="330"/>
+      <c r="J35" s="330"/>
+      <c r="K35" s="330"/>
       <c r="L35" s="323" t="s">
         <v>119</v>
       </c>
-      <c r="M35" s="322"/>
-      <c r="N35" s="322"/>
-      <c r="O35" s="324"/>
-      <c r="P35" s="303"/>
-      <c r="Q35" s="304"/>
-      <c r="R35" s="304"/>
-      <c r="S35" s="305"/>
-      <c r="T35" s="303" t="s">
+      <c r="M35" s="330"/>
+      <c r="N35" s="330"/>
+      <c r="O35" s="331"/>
+      <c r="P35" s="313"/>
+      <c r="Q35" s="314"/>
+      <c r="R35" s="314"/>
+      <c r="S35" s="315"/>
+      <c r="T35" s="313" t="s">
         <v>120</v>
       </c>
-      <c r="U35" s="304"/>
-      <c r="V35" s="304"/>
-      <c r="W35" s="305"/>
-      <c r="X35" s="303" t="s">
+      <c r="U35" s="314"/>
+      <c r="V35" s="314"/>
+      <c r="W35" s="315"/>
+      <c r="X35" s="313" t="s">
         <v>121</v>
       </c>
-      <c r="Y35" s="304"/>
-      <c r="Z35" s="304"/>
-      <c r="AA35" s="305"/>
+      <c r="Y35" s="314"/>
+      <c r="Z35" s="314"/>
+      <c r="AA35" s="315"/>
       <c r="AB35" s="107" t="s">
         <v>122</v>
       </c>
@@ -4479,26 +4473,26 @@
       <c r="M37" s="41"/>
       <c r="N37" s="27"/>
       <c r="O37" s="42"/>
-      <c r="P37" s="338"/>
-      <c r="Q37" s="340"/>
-      <c r="R37" s="340"/>
-      <c r="S37" s="339"/>
-      <c r="T37" s="343" t="s">
+      <c r="P37" s="306"/>
+      <c r="Q37" s="307"/>
+      <c r="R37" s="307"/>
+      <c r="S37" s="312"/>
+      <c r="T37" s="342" t="s">
         <v>127</v>
       </c>
-      <c r="U37" s="336"/>
-      <c r="V37" s="336"/>
-      <c r="W37" s="337"/>
-      <c r="X37" s="338" t="s">
+      <c r="U37" s="318"/>
+      <c r="V37" s="318"/>
+      <c r="W37" s="319"/>
+      <c r="X37" s="306" t="s">
         <v>128</v>
       </c>
-      <c r="Y37" s="340"/>
-      <c r="Z37" s="340"/>
-      <c r="AA37" s="339"/>
-      <c r="AB37" s="389"/>
-      <c r="AC37" s="390"/>
-      <c r="AD37" s="390"/>
-      <c r="AE37" s="391"/>
+      <c r="Y37" s="307"/>
+      <c r="Z37" s="307"/>
+      <c r="AA37" s="312"/>
+      <c r="AB37" s="370"/>
+      <c r="AC37" s="371"/>
+      <c r="AD37" s="371"/>
+      <c r="AE37" s="372"/>
     </row>
     <row r="38" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="86" t="s">
@@ -4531,27 +4525,27 @@
       <c r="N38" s="31"/>
       <c r="O38" s="32"/>
       <c r="P38" s="33"/>
-      <c r="Q38" s="392"/>
-      <c r="R38" s="392"/>
+      <c r="Q38" s="373"/>
+      <c r="R38" s="373"/>
       <c r="S38" s="35"/>
-      <c r="T38" s="393" t="s">
+      <c r="T38" s="358" t="s">
         <v>91</v>
       </c>
-      <c r="U38" s="394"/>
-      <c r="V38" s="394"/>
-      <c r="W38" s="395"/>
-      <c r="X38" s="396" t="s">
+      <c r="U38" s="359"/>
+      <c r="V38" s="359"/>
+      <c r="W38" s="360"/>
+      <c r="X38" s="374" t="s">
         <v>129</v>
       </c>
-      <c r="Y38" s="397"/>
-      <c r="Z38" s="397"/>
-      <c r="AA38" s="398"/>
-      <c r="AB38" s="399" t="s">
+      <c r="Y38" s="375"/>
+      <c r="Z38" s="375"/>
+      <c r="AA38" s="376"/>
+      <c r="AB38" s="377" t="s">
         <v>130</v>
       </c>
-      <c r="AC38" s="400"/>
-      <c r="AD38" s="400"/>
-      <c r="AE38" s="401"/>
+      <c r="AC38" s="378"/>
+      <c r="AD38" s="378"/>
+      <c r="AE38" s="379"/>
     </row>
     <row r="39" spans="1:31" s="79" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="86" t="s">
@@ -4575,18 +4569,18 @@
       <c r="Q39" s="45"/>
       <c r="R39" s="53"/>
       <c r="S39" s="35"/>
-      <c r="T39" s="383"/>
-      <c r="U39" s="384"/>
-      <c r="V39" s="384"/>
-      <c r="W39" s="385"/>
+      <c r="T39" s="345"/>
+      <c r="U39" s="346"/>
+      <c r="V39" s="346"/>
+      <c r="W39" s="347"/>
       <c r="X39" s="55"/>
       <c r="Y39" s="45"/>
       <c r="Z39" s="53"/>
       <c r="AA39" s="119"/>
-      <c r="AB39" s="386"/>
-      <c r="AC39" s="387"/>
-      <c r="AD39" s="387"/>
-      <c r="AE39" s="388"/>
+      <c r="AB39" s="367"/>
+      <c r="AC39" s="368"/>
+      <c r="AD39" s="368"/>
+      <c r="AE39" s="369"/>
     </row>
     <row r="40" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="101" t="s">
@@ -4651,28 +4645,28 @@
       <c r="G41" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="H41" s="321"/>
-      <c r="I41" s="359"/>
-      <c r="J41" s="359"/>
-      <c r="K41" s="359"/>
-      <c r="L41" s="359"/>
-      <c r="M41" s="359"/>
-      <c r="N41" s="359"/>
-      <c r="O41" s="409"/>
-      <c r="P41" s="303"/>
-      <c r="Q41" s="304"/>
-      <c r="R41" s="304"/>
-      <c r="S41" s="305"/>
-      <c r="T41" s="303"/>
-      <c r="U41" s="304"/>
-      <c r="V41" s="304"/>
-      <c r="W41" s="305"/>
+      <c r="H41" s="329"/>
+      <c r="I41" s="324"/>
+      <c r="J41" s="324"/>
+      <c r="K41" s="324"/>
+      <c r="L41" s="324"/>
+      <c r="M41" s="324"/>
+      <c r="N41" s="324"/>
+      <c r="O41" s="325"/>
+      <c r="P41" s="313"/>
+      <c r="Q41" s="314"/>
+      <c r="R41" s="314"/>
+      <c r="S41" s="315"/>
+      <c r="T41" s="313"/>
+      <c r="U41" s="314"/>
+      <c r="V41" s="314"/>
+      <c r="W41" s="315"/>
       <c r="X41" s="323" t="s">
         <v>137</v>
       </c>
-      <c r="Y41" s="359"/>
-      <c r="Z41" s="359"/>
-      <c r="AA41" s="409"/>
+      <c r="Y41" s="324"/>
+      <c r="Z41" s="324"/>
+      <c r="AA41" s="325"/>
       <c r="AB41" s="144"/>
       <c r="AC41" s="144"/>
       <c r="AD41" s="144"/>
@@ -4702,10 +4696,10 @@
       </c>
       <c r="H42" s="148"/>
       <c r="I42" s="31"/>
-      <c r="J42" s="340"/>
-      <c r="K42" s="340"/>
-      <c r="L42" s="340"/>
-      <c r="M42" s="340"/>
+      <c r="J42" s="307"/>
+      <c r="K42" s="307"/>
+      <c r="L42" s="307"/>
+      <c r="M42" s="307"/>
       <c r="N42" s="31"/>
       <c r="O42" s="34"/>
       <c r="P42" s="33"/>
@@ -4737,28 +4731,28 @@
       <c r="E43" s="39"/>
       <c r="F43" s="23"/>
       <c r="G43" s="90"/>
-      <c r="H43" s="408"/>
-      <c r="I43" s="340"/>
-      <c r="J43" s="340"/>
-      <c r="K43" s="340"/>
-      <c r="L43" s="340"/>
-      <c r="M43" s="340"/>
-      <c r="N43" s="340"/>
-      <c r="O43" s="339"/>
-      <c r="P43" s="338"/>
-      <c r="Q43" s="340"/>
-      <c r="R43" s="340"/>
-      <c r="S43" s="339"/>
-      <c r="T43" s="338"/>
-      <c r="U43" s="340"/>
-      <c r="V43" s="340"/>
-      <c r="W43" s="339"/>
-      <c r="X43" s="402" t="s">
+      <c r="H43" s="366"/>
+      <c r="I43" s="307"/>
+      <c r="J43" s="307"/>
+      <c r="K43" s="307"/>
+      <c r="L43" s="307"/>
+      <c r="M43" s="307"/>
+      <c r="N43" s="307"/>
+      <c r="O43" s="312"/>
+      <c r="P43" s="306"/>
+      <c r="Q43" s="307"/>
+      <c r="R43" s="307"/>
+      <c r="S43" s="312"/>
+      <c r="T43" s="306"/>
+      <c r="U43" s="307"/>
+      <c r="V43" s="307"/>
+      <c r="W43" s="312"/>
+      <c r="X43" s="320" t="s">
         <v>140</v>
       </c>
-      <c r="Y43" s="403"/>
-      <c r="Z43" s="403"/>
-      <c r="AA43" s="404"/>
+      <c r="Y43" s="321"/>
+      <c r="Z43" s="321"/>
+      <c r="AA43" s="322"/>
       <c r="AB43" s="156"/>
       <c r="AC43" s="157"/>
       <c r="AD43" s="156"/>
@@ -4815,14 +4809,14 @@
       <c r="E45" s="48"/>
       <c r="F45" s="49"/>
       <c r="G45" s="90"/>
-      <c r="H45" s="405"/>
-      <c r="I45" s="406"/>
-      <c r="J45" s="406"/>
-      <c r="K45" s="406"/>
-      <c r="L45" s="406"/>
-      <c r="M45" s="406"/>
-      <c r="N45" s="406"/>
-      <c r="O45" s="407"/>
+      <c r="H45" s="363"/>
+      <c r="I45" s="364"/>
+      <c r="J45" s="364"/>
+      <c r="K45" s="364"/>
+      <c r="L45" s="364"/>
+      <c r="M45" s="364"/>
+      <c r="N45" s="364"/>
+      <c r="O45" s="365"/>
       <c r="P45" s="55"/>
       <c r="Q45" s="45"/>
       <c r="R45" s="53"/>
@@ -4925,40 +4919,40 @@
       <c r="G48" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H48" s="321" t="s">
+      <c r="H48" s="329" t="s">
         <v>142</v>
       </c>
-      <c r="I48" s="322"/>
-      <c r="J48" s="322"/>
-      <c r="K48" s="322"/>
-      <c r="L48" s="429" t="s">
+      <c r="I48" s="330"/>
+      <c r="J48" s="330"/>
+      <c r="K48" s="330"/>
+      <c r="L48" s="303" t="s">
         <v>142</v>
       </c>
       <c r="M48" s="301"/>
       <c r="N48" s="301"/>
       <c r="O48" s="302"/>
-      <c r="P48" s="309" t="s">
+      <c r="P48" s="354" t="s">
         <v>143</v>
       </c>
-      <c r="Q48" s="411"/>
-      <c r="R48" s="411"/>
-      <c r="S48" s="412"/>
-      <c r="T48" s="303" t="s">
+      <c r="Q48" s="355"/>
+      <c r="R48" s="355"/>
+      <c r="S48" s="356"/>
+      <c r="T48" s="313" t="s">
         <v>144</v>
       </c>
-      <c r="U48" s="304"/>
-      <c r="V48" s="304"/>
-      <c r="W48" s="305"/>
-      <c r="X48" s="303"/>
-      <c r="Y48" s="304"/>
-      <c r="Z48" s="304"/>
-      <c r="AA48" s="305"/>
-      <c r="AB48" s="345" t="s">
+      <c r="U48" s="314"/>
+      <c r="V48" s="314"/>
+      <c r="W48" s="315"/>
+      <c r="X48" s="313"/>
+      <c r="Y48" s="314"/>
+      <c r="Z48" s="314"/>
+      <c r="AA48" s="315"/>
+      <c r="AB48" s="339" t="s">
         <v>145</v>
       </c>
-      <c r="AC48" s="346"/>
-      <c r="AD48" s="346"/>
-      <c r="AE48" s="410"/>
+      <c r="AC48" s="326"/>
+      <c r="AD48" s="326"/>
+      <c r="AE48" s="327"/>
     </row>
     <row r="49" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
@@ -5028,27 +5022,27 @@
       <c r="N50" s="27"/>
       <c r="O50" s="42"/>
       <c r="P50" s="186"/>
-      <c r="Q50" s="414" t="s">
+      <c r="Q50" s="362" t="s">
         <v>149</v>
       </c>
-      <c r="R50" s="414"/>
+      <c r="R50" s="362"/>
       <c r="S50" s="187"/>
-      <c r="T50" s="343" t="s">
+      <c r="T50" s="342" t="s">
         <v>150</v>
       </c>
-      <c r="U50" s="336"/>
-      <c r="V50" s="336"/>
-      <c r="W50" s="337"/>
-      <c r="X50" s="338"/>
-      <c r="Y50" s="340"/>
-      <c r="Z50" s="340"/>
-      <c r="AA50" s="339"/>
-      <c r="AB50" s="343" t="s">
+      <c r="U50" s="318"/>
+      <c r="V50" s="318"/>
+      <c r="W50" s="319"/>
+      <c r="X50" s="306"/>
+      <c r="Y50" s="307"/>
+      <c r="Z50" s="307"/>
+      <c r="AA50" s="312"/>
+      <c r="AB50" s="342" t="s">
         <v>146</v>
       </c>
-      <c r="AC50" s="336"/>
-      <c r="AD50" s="336"/>
-      <c r="AE50" s="344"/>
+      <c r="AC50" s="318"/>
+      <c r="AD50" s="318"/>
+      <c r="AE50" s="357"/>
     </row>
     <row r="51" spans="1:31" s="79" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25" t="s">
@@ -5086,22 +5080,22 @@
       <c r="Q51" s="80"/>
       <c r="R51" s="80"/>
       <c r="S51" s="187"/>
-      <c r="T51" s="393" t="s">
+      <c r="T51" s="358" t="s">
         <v>151</v>
       </c>
-      <c r="U51" s="394"/>
-      <c r="V51" s="394"/>
-      <c r="W51" s="395"/>
-      <c r="X51" s="353"/>
-      <c r="Y51" s="353"/>
-      <c r="Z51" s="353"/>
-      <c r="AA51" s="354"/>
-      <c r="AB51" s="393" t="s">
+      <c r="U51" s="359"/>
+      <c r="V51" s="359"/>
+      <c r="W51" s="360"/>
+      <c r="X51" s="335"/>
+      <c r="Y51" s="335"/>
+      <c r="Z51" s="335"/>
+      <c r="AA51" s="311"/>
+      <c r="AB51" s="358" t="s">
         <v>153</v>
       </c>
-      <c r="AC51" s="394"/>
-      <c r="AD51" s="394"/>
-      <c r="AE51" s="413"/>
+      <c r="AC51" s="359"/>
+      <c r="AD51" s="359"/>
+      <c r="AE51" s="361"/>
     </row>
     <row r="52" spans="1:31" s="79" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
@@ -5125,18 +5119,18 @@
       <c r="Q52" s="80"/>
       <c r="R52" s="183"/>
       <c r="S52" s="187"/>
-      <c r="T52" s="383"/>
-      <c r="U52" s="384"/>
-      <c r="V52" s="384"/>
-      <c r="W52" s="385"/>
+      <c r="T52" s="345"/>
+      <c r="U52" s="346"/>
+      <c r="V52" s="346"/>
+      <c r="W52" s="347"/>
       <c r="X52" s="55"/>
       <c r="Y52" s="45"/>
       <c r="Z52" s="53"/>
       <c r="AA52" s="119"/>
-      <c r="AB52" s="334"/>
-      <c r="AC52" s="384"/>
-      <c r="AD52" s="384"/>
-      <c r="AE52" s="415"/>
+      <c r="AB52" s="309"/>
+      <c r="AC52" s="346"/>
+      <c r="AD52" s="346"/>
+      <c r="AE52" s="348"/>
     </row>
     <row r="53" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="61"/>
@@ -5195,12 +5189,12 @@
       <c r="G54" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="321" t="s">
+      <c r="H54" s="329" t="s">
         <v>159</v>
       </c>
-      <c r="I54" s="322"/>
-      <c r="J54" s="322"/>
-      <c r="K54" s="324"/>
+      <c r="I54" s="330"/>
+      <c r="J54" s="330"/>
+      <c r="K54" s="331"/>
       <c r="L54" s="197" t="s">
         <v>160</v>
       </c>
@@ -5209,28 +5203,28 @@
         <v>161</v>
       </c>
       <c r="O54" s="199"/>
-      <c r="P54" s="303" t="s">
+      <c r="P54" s="313" t="s">
         <v>162</v>
       </c>
-      <c r="Q54" s="304"/>
-      <c r="R54" s="304"/>
-      <c r="S54" s="305"/>
-      <c r="T54" s="303" t="s">
+      <c r="Q54" s="314"/>
+      <c r="R54" s="314"/>
+      <c r="S54" s="315"/>
+      <c r="T54" s="313" t="s">
         <v>163</v>
       </c>
-      <c r="U54" s="304"/>
-      <c r="V54" s="304"/>
-      <c r="W54" s="305"/>
-      <c r="X54" s="345" t="s">
+      <c r="U54" s="314"/>
+      <c r="V54" s="314"/>
+      <c r="W54" s="315"/>
+      <c r="X54" s="339" t="s">
         <v>164</v>
       </c>
-      <c r="Y54" s="346"/>
-      <c r="Z54" s="346"/>
-      <c r="AA54" s="347"/>
-      <c r="AB54" s="303" t="s">
+      <c r="Y54" s="326"/>
+      <c r="Z54" s="326"/>
+      <c r="AA54" s="344"/>
+      <c r="AB54" s="313" t="s">
         <v>162</v>
       </c>
-      <c r="AC54" s="423"/>
+      <c r="AC54" s="343"/>
       <c r="AD54" s="200" t="s">
         <v>79</v>
       </c>
@@ -5307,24 +5301,24 @@
         <v>168</v>
       </c>
       <c r="O56" s="42"/>
-      <c r="P56" s="338" t="s">
+      <c r="P56" s="306" t="s">
         <v>169</v>
       </c>
-      <c r="Q56" s="340"/>
-      <c r="R56" s="340"/>
-      <c r="S56" s="339"/>
-      <c r="T56" s="343" t="s">
+      <c r="Q56" s="307"/>
+      <c r="R56" s="307"/>
+      <c r="S56" s="312"/>
+      <c r="T56" s="342" t="s">
         <v>170</v>
       </c>
-      <c r="U56" s="336"/>
-      <c r="V56" s="336"/>
-      <c r="W56" s="337"/>
-      <c r="X56" s="338" t="s">
+      <c r="U56" s="318"/>
+      <c r="V56" s="318"/>
+      <c r="W56" s="319"/>
+      <c r="X56" s="306" t="s">
         <v>171</v>
       </c>
-      <c r="Y56" s="340"/>
-      <c r="Z56" s="340"/>
-      <c r="AA56" s="339"/>
+      <c r="Y56" s="307"/>
+      <c r="Z56" s="307"/>
+      <c r="AA56" s="312"/>
       <c r="AB56" s="208" t="s">
         <v>172</v>
       </c>
@@ -5368,24 +5362,24 @@
         <v>152</v>
       </c>
       <c r="O57" s="42"/>
-      <c r="P57" s="330" t="s">
+      <c r="P57" s="341" t="s">
         <v>69</v>
       </c>
-      <c r="Q57" s="331"/>
-      <c r="R57" s="331"/>
-      <c r="S57" s="331"/>
-      <c r="T57" s="367" t="s">
+      <c r="Q57" s="310"/>
+      <c r="R57" s="310"/>
+      <c r="S57" s="310"/>
+      <c r="T57" s="332" t="s">
         <v>176</v>
       </c>
-      <c r="U57" s="418"/>
-      <c r="V57" s="418"/>
-      <c r="W57" s="419"/>
-      <c r="X57" s="379" t="s">
+      <c r="U57" s="333"/>
+      <c r="V57" s="333"/>
+      <c r="W57" s="334"/>
+      <c r="X57" s="351" t="s">
         <v>37</v>
       </c>
-      <c r="Y57" s="380"/>
-      <c r="Z57" s="380"/>
-      <c r="AA57" s="381"/>
+      <c r="Y57" s="352"/>
+      <c r="Z57" s="352"/>
+      <c r="AA57" s="353"/>
       <c r="AB57" s="213" t="s">
         <v>69</v>
       </c>
@@ -5417,10 +5411,10 @@
       <c r="Q58" s="45"/>
       <c r="R58" s="53"/>
       <c r="S58" s="35"/>
-      <c r="T58" s="420"/>
-      <c r="U58" s="421"/>
-      <c r="V58" s="421"/>
-      <c r="W58" s="422"/>
+      <c r="T58" s="336"/>
+      <c r="U58" s="337"/>
+      <c r="V58" s="337"/>
+      <c r="W58" s="338"/>
       <c r="X58" s="81"/>
       <c r="Y58" s="82"/>
       <c r="Z58" s="79"/>
@@ -5495,38 +5489,38 @@
       <c r="G60" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H60" s="321" t="s">
+      <c r="H60" s="329" t="s">
         <v>182</v>
       </c>
-      <c r="I60" s="322"/>
-      <c r="J60" s="322"/>
-      <c r="K60" s="322"/>
+      <c r="I60" s="330"/>
+      <c r="J60" s="330"/>
+      <c r="K60" s="330"/>
       <c r="L60" s="323" t="s">
         <v>182</v>
       </c>
-      <c r="M60" s="322"/>
-      <c r="N60" s="322"/>
-      <c r="O60" s="324"/>
-      <c r="P60" s="303" t="s">
+      <c r="M60" s="330"/>
+      <c r="N60" s="330"/>
+      <c r="O60" s="331"/>
+      <c r="P60" s="313" t="s">
         <v>183</v>
       </c>
-      <c r="Q60" s="304"/>
-      <c r="R60" s="304"/>
-      <c r="S60" s="305"/>
-      <c r="T60" s="303" t="s">
+      <c r="Q60" s="314"/>
+      <c r="R60" s="314"/>
+      <c r="S60" s="315"/>
+      <c r="T60" s="313" t="s">
         <v>184</v>
       </c>
-      <c r="U60" s="304"/>
-      <c r="V60" s="304"/>
-      <c r="W60" s="305"/>
-      <c r="X60" s="303" t="s">
+      <c r="U60" s="314"/>
+      <c r="V60" s="314"/>
+      <c r="W60" s="315"/>
+      <c r="X60" s="313" t="s">
         <v>158</v>
       </c>
-      <c r="Y60" s="304"/>
-      <c r="Z60" s="304"/>
-      <c r="AA60" s="305"/>
-      <c r="AB60" s="416"/>
-      <c r="AC60" s="417"/>
+      <c r="Y60" s="314"/>
+      <c r="Z60" s="314"/>
+      <c r="AA60" s="315"/>
+      <c r="AB60" s="349"/>
+      <c r="AC60" s="350"/>
       <c r="AD60" s="221"/>
       <c r="AE60" s="222"/>
     </row>
@@ -5596,24 +5590,24 @@
       <c r="M62" s="41"/>
       <c r="N62" s="27"/>
       <c r="O62" s="42"/>
-      <c r="P62" s="338" t="s">
+      <c r="P62" s="306" t="s">
         <v>187</v>
       </c>
-      <c r="Q62" s="340"/>
-      <c r="R62" s="340"/>
-      <c r="S62" s="339"/>
-      <c r="T62" s="338" t="s">
+      <c r="Q62" s="307"/>
+      <c r="R62" s="307"/>
+      <c r="S62" s="312"/>
+      <c r="T62" s="306" t="s">
         <v>188</v>
       </c>
-      <c r="U62" s="340"/>
-      <c r="V62" s="340"/>
-      <c r="W62" s="339"/>
-      <c r="X62" s="338" t="s">
+      <c r="U62" s="307"/>
+      <c r="V62" s="307"/>
+      <c r="W62" s="312"/>
+      <c r="X62" s="306" t="s">
         <v>189</v>
       </c>
-      <c r="Y62" s="340"/>
-      <c r="Z62" s="340"/>
-      <c r="AA62" s="339"/>
+      <c r="Y62" s="307"/>
+      <c r="Z62" s="307"/>
+      <c r="AA62" s="312"/>
       <c r="AB62" s="227"/>
       <c r="AC62" s="228"/>
       <c r="AD62" s="229"/>
@@ -5651,24 +5645,24 @@
       </c>
       <c r="N63" s="31"/>
       <c r="O63" s="32"/>
-      <c r="P63" s="330" t="s">
+      <c r="P63" s="341" t="s">
         <v>175</v>
       </c>
-      <c r="Q63" s="331"/>
-      <c r="R63" s="331"/>
-      <c r="S63" s="331"/>
+      <c r="Q63" s="310"/>
+      <c r="R63" s="310"/>
+      <c r="S63" s="310"/>
       <c r="T63" s="96"/>
-      <c r="U63" s="418" t="s">
+      <c r="U63" s="333" t="s">
         <v>112</v>
       </c>
-      <c r="V63" s="424"/>
+      <c r="V63" s="340"/>
       <c r="W63" s="234"/>
-      <c r="X63" s="330" t="s">
+      <c r="X63" s="341" t="s">
         <v>174</v>
       </c>
-      <c r="Y63" s="331"/>
-      <c r="Z63" s="331"/>
-      <c r="AA63" s="354"/>
+      <c r="Y63" s="310"/>
+      <c r="Z63" s="310"/>
+      <c r="AA63" s="311"/>
       <c r="AB63" s="235"/>
       <c r="AC63" s="236"/>
       <c r="AD63" s="237"/>
@@ -5764,42 +5758,42 @@
       <c r="G66" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H66" s="321" t="s">
+      <c r="H66" s="329" t="s">
         <v>192</v>
       </c>
-      <c r="I66" s="322"/>
-      <c r="J66" s="322"/>
-      <c r="K66" s="322"/>
+      <c r="I66" s="330"/>
+      <c r="J66" s="330"/>
+      <c r="K66" s="330"/>
       <c r="L66" s="323" t="s">
         <v>192</v>
       </c>
-      <c r="M66" s="322"/>
-      <c r="N66" s="322"/>
-      <c r="O66" s="324"/>
-      <c r="P66" s="345" t="s">
+      <c r="M66" s="330"/>
+      <c r="N66" s="330"/>
+      <c r="O66" s="331"/>
+      <c r="P66" s="339" t="s">
         <v>193</v>
       </c>
-      <c r="Q66" s="346"/>
-      <c r="R66" s="346"/>
-      <c r="S66" s="346"/>
-      <c r="T66" s="303" t="s">
+      <c r="Q66" s="326"/>
+      <c r="R66" s="326"/>
+      <c r="S66" s="326"/>
+      <c r="T66" s="313" t="s">
         <v>84</v>
       </c>
-      <c r="U66" s="304"/>
-      <c r="V66" s="304"/>
-      <c r="W66" s="305"/>
-      <c r="X66" s="303" t="s">
+      <c r="U66" s="314"/>
+      <c r="V66" s="314"/>
+      <c r="W66" s="315"/>
+      <c r="X66" s="313" t="s">
         <v>194</v>
       </c>
-      <c r="Y66" s="304"/>
-      <c r="Z66" s="304"/>
-      <c r="AA66" s="305"/>
-      <c r="AB66" s="303" t="s">
+      <c r="Y66" s="314"/>
+      <c r="Z66" s="314"/>
+      <c r="AA66" s="315"/>
+      <c r="AB66" s="313" t="s">
         <v>195</v>
       </c>
-      <c r="AC66" s="304"/>
-      <c r="AD66" s="304"/>
-      <c r="AE66" s="427"/>
+      <c r="AC66" s="314"/>
+      <c r="AD66" s="314"/>
+      <c r="AE66" s="316"/>
     </row>
     <row r="67" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
@@ -5869,29 +5863,29 @@
       <c r="N68" s="27"/>
       <c r="O68" s="42"/>
       <c r="P68" s="33"/>
-      <c r="Q68" s="340" t="s">
+      <c r="Q68" s="307" t="s">
         <v>198</v>
       </c>
-      <c r="R68" s="340"/>
+      <c r="R68" s="307"/>
       <c r="S68" s="35"/>
-      <c r="T68" s="343" t="s">
+      <c r="T68" s="342" t="s">
         <v>199</v>
       </c>
-      <c r="U68" s="336"/>
-      <c r="V68" s="336"/>
-      <c r="W68" s="337"/>
-      <c r="X68" s="338" t="s">
+      <c r="U68" s="318"/>
+      <c r="V68" s="318"/>
+      <c r="W68" s="319"/>
+      <c r="X68" s="306" t="s">
         <v>200</v>
       </c>
-      <c r="Y68" s="340"/>
-      <c r="Z68" s="340"/>
-      <c r="AA68" s="339"/>
-      <c r="AB68" s="338" t="s">
+      <c r="Y68" s="307"/>
+      <c r="Z68" s="307"/>
+      <c r="AA68" s="312"/>
+      <c r="AB68" s="306" t="s">
         <v>201</v>
       </c>
-      <c r="AC68" s="340"/>
-      <c r="AD68" s="340"/>
-      <c r="AE68" s="425"/>
+      <c r="AC68" s="307"/>
+      <c r="AD68" s="307"/>
+      <c r="AE68" s="308"/>
     </row>
     <row r="69" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
@@ -5926,25 +5920,25 @@
       <c r="N69" s="31"/>
       <c r="O69" s="32"/>
       <c r="P69" s="33"/>
-      <c r="Q69" s="426" t="s">
+      <c r="Q69" s="328" t="s">
         <v>111</v>
       </c>
-      <c r="R69" s="426"/>
+      <c r="R69" s="328"/>
       <c r="S69" s="35"/>
-      <c r="T69" s="367" t="s">
+      <c r="T69" s="332" t="s">
         <v>203</v>
       </c>
-      <c r="U69" s="418"/>
-      <c r="V69" s="418"/>
-      <c r="W69" s="419"/>
-      <c r="X69" s="353" t="s">
+      <c r="U69" s="333"/>
+      <c r="V69" s="333"/>
+      <c r="W69" s="334"/>
+      <c r="X69" s="335" t="s">
         <v>204</v>
       </c>
-      <c r="Y69" s="353"/>
-      <c r="Z69" s="353"/>
-      <c r="AA69" s="354"/>
+      <c r="Y69" s="335"/>
+      <c r="Z69" s="335"/>
+      <c r="AA69" s="311"/>
       <c r="AB69" s="33"/>
-      <c r="AC69" s="431" t="s">
+      <c r="AC69" s="305" t="s">
         <v>66</v>
       </c>
       <c r="AD69" s="31"/>
@@ -5972,10 +5966,10 @@
       <c r="Q70" s="45"/>
       <c r="R70" s="53"/>
       <c r="S70" s="35"/>
-      <c r="T70" s="420"/>
-      <c r="U70" s="421"/>
-      <c r="V70" s="421"/>
-      <c r="W70" s="422"/>
+      <c r="T70" s="336"/>
+      <c r="U70" s="337"/>
+      <c r="V70" s="337"/>
+      <c r="W70" s="338"/>
       <c r="X70" s="55"/>
       <c r="Y70" s="45"/>
       <c r="Z70" s="53"/>
@@ -6046,38 +6040,38 @@
       <c r="G72" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H72" s="321" t="s">
+      <c r="H72" s="329" t="s">
         <v>209</v>
       </c>
-      <c r="I72" s="322"/>
-      <c r="J72" s="322"/>
-      <c r="K72" s="322"/>
+      <c r="I72" s="330"/>
+      <c r="J72" s="330"/>
+      <c r="K72" s="330"/>
       <c r="L72" s="323" t="s">
         <v>209</v>
       </c>
-      <c r="M72" s="322"/>
-      <c r="N72" s="322"/>
-      <c r="O72" s="324"/>
-      <c r="P72" s="303"/>
-      <c r="Q72" s="304"/>
-      <c r="R72" s="304"/>
-      <c r="S72" s="305"/>
-      <c r="T72" s="303" t="s">
+      <c r="M72" s="330"/>
+      <c r="N72" s="330"/>
+      <c r="O72" s="331"/>
+      <c r="P72" s="313"/>
+      <c r="Q72" s="314"/>
+      <c r="R72" s="314"/>
+      <c r="S72" s="315"/>
+      <c r="T72" s="313" t="s">
         <v>210</v>
       </c>
-      <c r="U72" s="304"/>
-      <c r="V72" s="304"/>
-      <c r="W72" s="305"/>
-      <c r="X72" s="303" t="s">
+      <c r="U72" s="314"/>
+      <c r="V72" s="314"/>
+      <c r="W72" s="315"/>
+      <c r="X72" s="313" t="s">
         <v>211</v>
       </c>
-      <c r="Y72" s="304"/>
-      <c r="Z72" s="304"/>
-      <c r="AA72" s="305"/>
-      <c r="AB72" s="303"/>
-      <c r="AC72" s="304"/>
-      <c r="AD72" s="304"/>
-      <c r="AE72" s="427"/>
+      <c r="Y72" s="314"/>
+      <c r="Z72" s="314"/>
+      <c r="AA72" s="315"/>
+      <c r="AB72" s="313"/>
+      <c r="AC72" s="314"/>
+      <c r="AD72" s="314"/>
+      <c r="AE72" s="316"/>
     </row>
     <row r="73" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="25" t="s">
@@ -6146,26 +6140,26 @@
       <c r="M74" s="41"/>
       <c r="N74" s="27"/>
       <c r="O74" s="42"/>
-      <c r="P74" s="338"/>
-      <c r="Q74" s="340"/>
-      <c r="R74" s="340"/>
-      <c r="S74" s="339"/>
-      <c r="T74" s="338" t="s">
+      <c r="P74" s="306"/>
+      <c r="Q74" s="307"/>
+      <c r="R74" s="307"/>
+      <c r="S74" s="312"/>
+      <c r="T74" s="306" t="s">
         <v>214</v>
       </c>
-      <c r="U74" s="340"/>
-      <c r="V74" s="340"/>
-      <c r="W74" s="339"/>
-      <c r="X74" s="338" t="s">
+      <c r="U74" s="307"/>
+      <c r="V74" s="307"/>
+      <c r="W74" s="312"/>
+      <c r="X74" s="306" t="s">
         <v>215</v>
       </c>
-      <c r="Y74" s="340"/>
-      <c r="Z74" s="340"/>
-      <c r="AA74" s="339"/>
-      <c r="AB74" s="338"/>
-      <c r="AC74" s="340"/>
-      <c r="AD74" s="340"/>
-      <c r="AE74" s="425"/>
+      <c r="Y74" s="307"/>
+      <c r="Z74" s="307"/>
+      <c r="AA74" s="312"/>
+      <c r="AB74" s="306"/>
+      <c r="AC74" s="307"/>
+      <c r="AD74" s="307"/>
+      <c r="AE74" s="308"/>
     </row>
     <row r="75" spans="1:31" s="79" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
@@ -6209,12 +6203,12 @@
       </c>
       <c r="V75" s="253"/>
       <c r="W75" s="250"/>
-      <c r="X75" s="334" t="s">
+      <c r="X75" s="309" t="s">
         <v>218</v>
       </c>
-      <c r="Y75" s="331"/>
-      <c r="Z75" s="331"/>
-      <c r="AA75" s="354"/>
+      <c r="Y75" s="310"/>
+      <c r="Z75" s="310"/>
+      <c r="AA75" s="311"/>
       <c r="AB75" s="33"/>
       <c r="AC75" s="29"/>
       <c r="AD75" s="31"/>
@@ -6314,10 +6308,10 @@
       </c>
       <c r="H78" s="261"/>
       <c r="I78" s="262"/>
-      <c r="J78" s="304"/>
-      <c r="K78" s="304"/>
-      <c r="L78" s="304"/>
-      <c r="M78" s="304"/>
+      <c r="J78" s="314"/>
+      <c r="K78" s="314"/>
+      <c r="L78" s="314"/>
+      <c r="M78" s="314"/>
       <c r="N78" s="263"/>
       <c r="O78" s="264"/>
       <c r="P78" s="265"/>
@@ -6329,13 +6323,13 @@
       <c r="V78" s="271"/>
       <c r="W78" s="272"/>
       <c r="X78" s="323"/>
-      <c r="Y78" s="359"/>
-      <c r="Z78" s="359"/>
-      <c r="AA78" s="409"/>
-      <c r="AB78" s="346"/>
-      <c r="AC78" s="346"/>
-      <c r="AD78" s="346"/>
-      <c r="AE78" s="410"/>
+      <c r="Y78" s="324"/>
+      <c r="Z78" s="324"/>
+      <c r="AA78" s="325"/>
+      <c r="AB78" s="326"/>
+      <c r="AC78" s="326"/>
+      <c r="AD78" s="326"/>
+      <c r="AE78" s="327"/>
     </row>
     <row r="79" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
@@ -6393,14 +6387,14 @@
       <c r="E80" s="39"/>
       <c r="F80" s="23"/>
       <c r="G80" s="90"/>
-      <c r="H80" s="428"/>
-      <c r="I80" s="336"/>
-      <c r="J80" s="336"/>
-      <c r="K80" s="336"/>
-      <c r="L80" s="336"/>
-      <c r="M80" s="336"/>
-      <c r="N80" s="336"/>
-      <c r="O80" s="337"/>
+      <c r="H80" s="317"/>
+      <c r="I80" s="318"/>
+      <c r="J80" s="318"/>
+      <c r="K80" s="318"/>
+      <c r="L80" s="318"/>
+      <c r="M80" s="318"/>
+      <c r="N80" s="318"/>
+      <c r="O80" s="319"/>
       <c r="P80" s="280"/>
       <c r="Q80" s="281"/>
       <c r="R80" s="35"/>
@@ -6408,14 +6402,14 @@
       <c r="T80" s="96"/>
       <c r="U80" s="282"/>
       <c r="V80" s="97"/>
-      <c r="X80" s="402"/>
-      <c r="Y80" s="403"/>
-      <c r="Z80" s="403"/>
-      <c r="AA80" s="404"/>
-      <c r="AB80" s="340"/>
-      <c r="AC80" s="340"/>
-      <c r="AD80" s="340"/>
-      <c r="AE80" s="425"/>
+      <c r="X80" s="320"/>
+      <c r="Y80" s="321"/>
+      <c r="Z80" s="321"/>
+      <c r="AA80" s="322"/>
+      <c r="AB80" s="307"/>
+      <c r="AC80" s="307"/>
+      <c r="AD80" s="307"/>
+      <c r="AE80" s="308"/>
     </row>
     <row r="81" spans="1:31" s="13" customFormat="1" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="25" t="s">
@@ -6727,125 +6721,33 @@
     </row>
   </sheetData>
   <mergeCells count="167">
-    <mergeCell ref="AB74:AE74"/>
-    <mergeCell ref="X75:AA75"/>
-    <mergeCell ref="P74:S74"/>
-    <mergeCell ref="T74:W74"/>
-    <mergeCell ref="X74:AA74"/>
-    <mergeCell ref="T72:W72"/>
-    <mergeCell ref="X72:AA72"/>
-    <mergeCell ref="AB72:AE72"/>
-    <mergeCell ref="H80:O80"/>
-    <mergeCell ref="X80:AA80"/>
-    <mergeCell ref="AB80:AE80"/>
-    <mergeCell ref="J78:M78"/>
-    <mergeCell ref="X78:AA78"/>
-    <mergeCell ref="AB78:AE78"/>
-    <mergeCell ref="AB68:AE68"/>
-    <mergeCell ref="Q69:R69"/>
-    <mergeCell ref="X66:AA66"/>
-    <mergeCell ref="AB66:AE66"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="L72:O72"/>
-    <mergeCell ref="P72:S72"/>
-    <mergeCell ref="T69:W69"/>
-    <mergeCell ref="X69:AA69"/>
-    <mergeCell ref="T70:W70"/>
-    <mergeCell ref="H66:K66"/>
-    <mergeCell ref="L66:O66"/>
-    <mergeCell ref="P66:S66"/>
-    <mergeCell ref="T66:W66"/>
-    <mergeCell ref="U63:V63"/>
-    <mergeCell ref="X63:AA63"/>
-    <mergeCell ref="Q68:R68"/>
-    <mergeCell ref="T68:W68"/>
-    <mergeCell ref="X68:AA68"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="T62:W62"/>
-    <mergeCell ref="X62:AA62"/>
-    <mergeCell ref="P63:S63"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="L60:O60"/>
-    <mergeCell ref="P60:S60"/>
-    <mergeCell ref="T60:W60"/>
-    <mergeCell ref="X60:AA60"/>
-    <mergeCell ref="AB54:AC54"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="P54:S54"/>
-    <mergeCell ref="T54:W54"/>
-    <mergeCell ref="X54:AA54"/>
-    <mergeCell ref="T52:W52"/>
-    <mergeCell ref="AB52:AE52"/>
-    <mergeCell ref="AB60:AC60"/>
-    <mergeCell ref="P57:S57"/>
-    <mergeCell ref="T57:W57"/>
-    <mergeCell ref="X57:AA57"/>
-    <mergeCell ref="T58:W58"/>
-    <mergeCell ref="P56:S56"/>
-    <mergeCell ref="T56:W56"/>
-    <mergeCell ref="X56:AA56"/>
-    <mergeCell ref="X48:AA48"/>
-    <mergeCell ref="AB48:AE48"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="P48:S48"/>
-    <mergeCell ref="T48:W48"/>
-    <mergeCell ref="AB50:AE50"/>
-    <mergeCell ref="T51:W51"/>
-    <mergeCell ref="X51:AA51"/>
-    <mergeCell ref="AB51:AE51"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="T50:W50"/>
-    <mergeCell ref="X50:AA50"/>
-    <mergeCell ref="X43:AA43"/>
-    <mergeCell ref="H45:O45"/>
-    <mergeCell ref="H43:O43"/>
-    <mergeCell ref="P43:S43"/>
-    <mergeCell ref="T43:W43"/>
-    <mergeCell ref="H41:O41"/>
-    <mergeCell ref="P41:S41"/>
-    <mergeCell ref="T41:W41"/>
-    <mergeCell ref="X41:AA41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="AB39:AE39"/>
-    <mergeCell ref="AB37:AE37"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="T38:W38"/>
-    <mergeCell ref="X38:AA38"/>
-    <mergeCell ref="AB38:AE38"/>
-    <mergeCell ref="P37:S37"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="X37:AA37"/>
-    <mergeCell ref="X35:AA35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="L35:O35"/>
-    <mergeCell ref="P35:S35"/>
-    <mergeCell ref="T35:W35"/>
-    <mergeCell ref="P32:S32"/>
-    <mergeCell ref="T32:W32"/>
-    <mergeCell ref="X32:AA32"/>
-    <mergeCell ref="T39:W39"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="P29:S29"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="T27:W27"/>
-    <mergeCell ref="AB28:AC28"/>
-    <mergeCell ref="P31:S31"/>
-    <mergeCell ref="T31:W31"/>
-    <mergeCell ref="X31:AA31"/>
-    <mergeCell ref="T29:W29"/>
-    <mergeCell ref="X29:AA29"/>
-    <mergeCell ref="P30:S30"/>
-    <mergeCell ref="X30:AA30"/>
-    <mergeCell ref="X24:AA24"/>
-    <mergeCell ref="AB24:AE24"/>
-    <mergeCell ref="AD28:AE28"/>
-    <mergeCell ref="P25:S25"/>
-    <mergeCell ref="T25:W25"/>
-    <mergeCell ref="X25:AA25"/>
-    <mergeCell ref="AB25:AE25"/>
-    <mergeCell ref="T26:W26"/>
-    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="X11:AA11"/>
+    <mergeCell ref="AB11:AE11"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB9:AE9"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="L14:O14"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="AB14:AE14"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="AD18:AE18"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:W13"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="AB13:AE13"/>
     <mergeCell ref="P19:S19"/>
     <mergeCell ref="T17:U17"/>
     <mergeCell ref="V17:W17"/>
@@ -6867,33 +6769,125 @@
     <mergeCell ref="X23:AA23"/>
     <mergeCell ref="AB23:AE23"/>
     <mergeCell ref="P17:S17"/>
-    <mergeCell ref="L14:O14"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="AB14:AE14"/>
-    <mergeCell ref="T15:W15"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="AD18:AE18"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="T13:W13"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB13:AE13"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="X11:AA11"/>
-    <mergeCell ref="AB11:AE11"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB9:AE9"/>
-    <mergeCell ref="AD12:AE12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="X24:AA24"/>
+    <mergeCell ref="AB24:AE24"/>
+    <mergeCell ref="AD28:AE28"/>
+    <mergeCell ref="P25:S25"/>
+    <mergeCell ref="T25:W25"/>
+    <mergeCell ref="X25:AA25"/>
+    <mergeCell ref="AB25:AE25"/>
+    <mergeCell ref="T26:W26"/>
+    <mergeCell ref="X26:AA26"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="P29:S29"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="T27:W27"/>
+    <mergeCell ref="AB28:AC28"/>
+    <mergeCell ref="P31:S31"/>
+    <mergeCell ref="T31:W31"/>
+    <mergeCell ref="X31:AA31"/>
+    <mergeCell ref="T29:W29"/>
+    <mergeCell ref="X29:AA29"/>
+    <mergeCell ref="P30:S30"/>
+    <mergeCell ref="X30:AA30"/>
+    <mergeCell ref="X35:AA35"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="L35:O35"/>
+    <mergeCell ref="P35:S35"/>
+    <mergeCell ref="T35:W35"/>
+    <mergeCell ref="P32:S32"/>
+    <mergeCell ref="T32:W32"/>
+    <mergeCell ref="X32:AA32"/>
+    <mergeCell ref="T39:W39"/>
+    <mergeCell ref="AB39:AE39"/>
+    <mergeCell ref="AB37:AE37"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="T38:W38"/>
+    <mergeCell ref="X38:AA38"/>
+    <mergeCell ref="AB38:AE38"/>
+    <mergeCell ref="P37:S37"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="X37:AA37"/>
+    <mergeCell ref="X43:AA43"/>
+    <mergeCell ref="H45:O45"/>
+    <mergeCell ref="H43:O43"/>
+    <mergeCell ref="P43:S43"/>
+    <mergeCell ref="T43:W43"/>
+    <mergeCell ref="H41:O41"/>
+    <mergeCell ref="P41:S41"/>
+    <mergeCell ref="T41:W41"/>
+    <mergeCell ref="X41:AA41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="X48:AA48"/>
+    <mergeCell ref="AB48:AE48"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="P48:S48"/>
+    <mergeCell ref="T48:W48"/>
+    <mergeCell ref="AB50:AE50"/>
+    <mergeCell ref="T51:W51"/>
+    <mergeCell ref="X51:AA51"/>
+    <mergeCell ref="AB51:AE51"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="T50:W50"/>
+    <mergeCell ref="X50:AA50"/>
+    <mergeCell ref="T52:W52"/>
+    <mergeCell ref="AB52:AE52"/>
+    <mergeCell ref="AB60:AC60"/>
+    <mergeCell ref="P57:S57"/>
+    <mergeCell ref="T57:W57"/>
+    <mergeCell ref="X57:AA57"/>
+    <mergeCell ref="T58:W58"/>
+    <mergeCell ref="P56:S56"/>
+    <mergeCell ref="T56:W56"/>
+    <mergeCell ref="X56:AA56"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="L60:O60"/>
+    <mergeCell ref="P60:S60"/>
+    <mergeCell ref="T60:W60"/>
+    <mergeCell ref="X60:AA60"/>
+    <mergeCell ref="AB54:AC54"/>
+    <mergeCell ref="H54:K54"/>
+    <mergeCell ref="P54:S54"/>
+    <mergeCell ref="T54:W54"/>
+    <mergeCell ref="X54:AA54"/>
+    <mergeCell ref="U63:V63"/>
+    <mergeCell ref="X63:AA63"/>
+    <mergeCell ref="Q68:R68"/>
+    <mergeCell ref="T68:W68"/>
+    <mergeCell ref="X68:AA68"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="T62:W62"/>
+    <mergeCell ref="X62:AA62"/>
+    <mergeCell ref="P63:S63"/>
+    <mergeCell ref="AB68:AE68"/>
+    <mergeCell ref="Q69:R69"/>
+    <mergeCell ref="X66:AA66"/>
+    <mergeCell ref="AB66:AE66"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="L72:O72"/>
+    <mergeCell ref="P72:S72"/>
+    <mergeCell ref="T69:W69"/>
+    <mergeCell ref="X69:AA69"/>
+    <mergeCell ref="T70:W70"/>
+    <mergeCell ref="H66:K66"/>
+    <mergeCell ref="L66:O66"/>
+    <mergeCell ref="P66:S66"/>
+    <mergeCell ref="T66:W66"/>
+    <mergeCell ref="AB74:AE74"/>
+    <mergeCell ref="X75:AA75"/>
+    <mergeCell ref="P74:S74"/>
+    <mergeCell ref="T74:W74"/>
+    <mergeCell ref="X74:AA74"/>
+    <mergeCell ref="T72:W72"/>
+    <mergeCell ref="X72:AA72"/>
+    <mergeCell ref="AB72:AE72"/>
+    <mergeCell ref="H80:O80"/>
+    <mergeCell ref="X80:AA80"/>
+    <mergeCell ref="AB80:AE80"/>
+    <mergeCell ref="J78:M78"/>
+    <mergeCell ref="X78:AA78"/>
+    <mergeCell ref="AB78:AE78"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="U63" r:id="rId1" display="oxabra@yandex.ru"/>

</xml_diff>